<commit_message>
added changes for Nabil to handle incorrect handles and better error handles
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umarh\projects\shopify_exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0491670D-E312-4F6D-BB3E-0A747EF13891}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22C5103-A597-4DEF-BA6A-F0AB3E0BFC78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="30960" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="30960" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,14 +363,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>